<commit_message>
CCD-4390 updated functional tests
CCD-4390 fixed checkstyle errors

CCD-4390 fixed unit test failures

CCD-4390 fixed unit test failures

CCD-4390 fixed BDD test failure

CCD-4390 fixed BDD test failure

CCD-4390 fixed BDD test failure

CCD-4390 fixed BDD test failure

CCD-4390 fixed BDD test failure
</commit_message>
<xml_diff>
--- a/aat/src/resource/CCD_CNP_27_Invalid_CaseRole.xlsx
+++ b/aat/src/resource/CCD_CNP_27_Invalid_CaseRole.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/support/ccd-definition-store-api/aat/src/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E98D52A-234E-1447-80FF-EE78FD4F474A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7805034E-6447-7842-8077-1EAB2C6F6F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1080" windowWidth="29180" windowHeight="16620" tabRatio="823" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2697" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2701" uniqueCount="301">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -964,6 +964,9 @@
   </si>
   <si>
     <t>[INTVRSOLICITOR2]</t>
+  </si>
+  <si>
+    <t>Intervener2's Solicitor</t>
   </si>
 </sst>
 </file>
@@ -9835,7 +9838,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9898,7 +9901,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>296</v>
@@ -9915,7 +9918,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>298</v>
@@ -9932,7 +9935,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>297</v>
@@ -11150,7 +11153,7 @@
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11222,16 +11225,33 @@
         <v>43466</v>
       </c>
       <c r="C4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D4" t="s">
-        <v>285</v>
+        <v>274</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>298</v>
       </c>
       <c r="E4" t="s">
         <v>286</v>
       </c>
       <c r="F4" t="s">
         <v>286</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>43466</v>
+      </c>
+      <c r="C5" t="s">
+        <v>274</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>300</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="17" spans="18:18" x14ac:dyDescent="0.15">
@@ -11246,8 +11266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>